<commit_message>
better z finding function + text file inpuit
Better z finding function that doesnt just mark everything as a hit also text z input is now possible
</commit_message>
<xml_diff>
--- a/output/ROC Curve 2 Compounds_processed_analysis.xlsx
+++ b/output/ROC Curve 2 Compounds_processed_analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="92">
   <si>
     <t>compound_id</t>
   </si>
@@ -269,16 +269,16 @@
     <t>F1 Score</t>
   </si>
   <si>
-    <t>AUC</t>
+    <t>Sweep</t>
+  </si>
+  <si>
+    <t>Optimal Z</t>
   </si>
   <si>
     <t>Input Z</t>
   </si>
   <si>
-    <t>Optimal Z (Min FN)</t>
-  </si>
-  <si>
-    <t>Compound G ROC (AUC=0.991)</t>
+    <t>Compound G ROC (AUC=0.9144736842105263)</t>
   </si>
   <si>
     <t>FPR</t>
@@ -287,7 +287,10 @@
     <t>TPR</t>
   </si>
   <si>
-    <t>Compound F ROC (AUC=0.953)</t>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Compound F ROC (AUC=0.8947368421052632)</t>
   </si>
   <si>
     <t>FPR_Chance</t>
@@ -381,7 +384,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>All Compounds ROC Curves (Curved Scatter)</a:t>
+              <a:t>All Compounds ROC Curves (User-defined z)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -396,131 +399,32 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Compound G (AUC=0.991)</c:v>
+            <c:v>Compound G</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400"/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="6"/>
+            <c:size val="7"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ROC_Curves!$A$3:$A$13</c:f>
+              <c:f>ROC_Curves!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.166667</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.166667</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>ROC_Curves!$B$3:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.052632</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.184211</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.289474</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.368421</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.684211</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.947368</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.947368</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Compound F (AUC=0.953)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400"/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="6"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>ROC_Curves!$A$18:$A$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.1666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -538,64 +442,211 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.166667</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.333333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.583333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ROC_Curves!$B$18:$B$30</c:f>
+              <c:f>ROC_Curves!$B$3:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9473684210526315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2894736842105263</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2894736842105263</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.05263157894736842</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Compound F</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ROC_Curves!$A$23:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.078947</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.236842</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.289474</c:v>
+                  <c:v>0.1666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.421053</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.526316</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.657895</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.710526</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.868421</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.868421</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.973684</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.973684</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ROC_Curves!$B$23:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.868421052631579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5263157894736842</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2368421052631579</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.07894736842105263</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.07894736842105263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -621,7 +672,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ROC_Curves!$K$39:$K$40</c:f>
+              <c:f>ROC_Curves!$Z$47:$Z$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -636,7 +687,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ROC_Curves!$L$39:$L$40</c:f>
+              <c:f>ROC_Curves!$AA$47:$AA$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -741,13 +792,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5530,7 +5581,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5538,17 +5589,17 @@
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="9" width="4.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="15" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -5591,11 +5642,8 @@
       <c r="N1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -5603,40 +5651,43 @@
         <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2">
-        <v>5.5</v>
+        <v>0.1</v>
       </c>
       <c r="E2">
-        <v>935</v>
+        <v>17</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>12</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0.24</v>
+        <v>0.76</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>0.9912280701754386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0.76</v>
+      </c>
+      <c r="N2">
+        <v>0.8636363636363636</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -5644,13 +5695,13 @@
         <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="F3">
         <v>38</v>
@@ -5679,96 +5730,1223 @@
       <c r="N3">
         <v>0.8636363636363636</v>
       </c>
-      <c r="O3">
-        <v>0.9912280701754386</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
         <v>83</v>
       </c>
       <c r="D4">
+        <v>0.8</v>
+      </c>
+      <c r="E4">
+        <v>136</v>
+      </c>
+      <c r="F4">
+        <v>38</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0.76</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0.76</v>
+      </c>
+      <c r="N4">
+        <v>0.8636363636363636</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>170</v>
+      </c>
+      <c r="F5">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0.92</v>
+      </c>
+      <c r="K5">
+        <v>0.9473684210526315</v>
+      </c>
+      <c r="L5">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="M5">
+        <v>0.9473684210526315</v>
+      </c>
+      <c r="N5">
+        <v>0.9473684210526315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>170</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6">
+        <v>255</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>27</v>
+      </c>
+      <c r="J6">
+        <v>0.46</v>
+      </c>
+      <c r="K6">
+        <v>0.2894736842105263</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0.4489795918367347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>340</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>27</v>
+      </c>
+      <c r="J7">
+        <v>0.46</v>
+      </c>
+      <c r="K7">
+        <v>0.2894736842105263</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0.4489795918367347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>170</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>2.5</v>
+      </c>
+      <c r="E8">
+        <v>425</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>36</v>
+      </c>
+      <c r="J8">
+        <v>0.28</v>
+      </c>
+      <c r="K8">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>170</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>510</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>38</v>
+      </c>
+      <c r="J9">
+        <v>0.24</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>170</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10">
+        <v>3.5</v>
+      </c>
+      <c r="E10">
+        <v>595</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>38</v>
+      </c>
+      <c r="J10">
+        <v>0.24</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>170</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>680</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
+      </c>
+      <c r="J11">
+        <v>0.24</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>170</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12">
+        <v>4.5</v>
+      </c>
+      <c r="E12">
+        <v>765</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>38</v>
+      </c>
+      <c r="J12">
+        <v>0.24</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>850</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>38</v>
+      </c>
+      <c r="J13">
+        <v>0.24</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>170</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14">
         <v>5.5</v>
       </c>
-      <c r="E4">
+      <c r="E14">
+        <v>935</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>38</v>
+      </c>
+      <c r="J14">
+        <v>0.24</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>170</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>1020</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>38</v>
+      </c>
+      <c r="J15">
+        <v>0.24</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>170</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16">
+        <v>6.5</v>
+      </c>
+      <c r="E16">
+        <v>1105</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>12</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>38</v>
+      </c>
+      <c r="J16">
+        <v>0.24</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>170</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>1190</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>38</v>
+      </c>
+      <c r="J17">
+        <v>0.24</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>164</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+      <c r="E18">
+        <v>16.4</v>
+      </c>
+      <c r="F18">
+        <v>38</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>12</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0.76</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0.76</v>
+      </c>
+      <c r="N18">
+        <v>0.8636363636363636</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>164</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+      <c r="E19">
+        <v>82</v>
+      </c>
+      <c r="F19">
+        <v>38</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0.76</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0.76</v>
+      </c>
+      <c r="N19">
+        <v>0.8636363636363636</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>164</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20">
+        <v>0.8</v>
+      </c>
+      <c r="E20">
+        <v>131.2</v>
+      </c>
+      <c r="F20">
+        <v>38</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0.76</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0.76</v>
+      </c>
+      <c r="N20">
+        <v>0.8636363636363636</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>164</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>164</v>
+      </c>
+      <c r="F21">
+        <v>33</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>0.86</v>
+      </c>
+      <c r="K21">
+        <v>0.868421052631579</v>
+      </c>
+      <c r="L21">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="M21">
+        <v>0.9428571428571428</v>
+      </c>
+      <c r="N21">
+        <v>0.904109589041096</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22">
+        <v>1.5</v>
+      </c>
+      <c r="E22">
+        <v>246</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22">
+        <v>12</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>18</v>
+      </c>
+      <c r="J22">
+        <v>0.64</v>
+      </c>
+      <c r="K22">
+        <v>0.5263157894736842</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>0.6896551724137931</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>164</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>328</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>29</v>
+      </c>
+      <c r="J23">
+        <v>0.42</v>
+      </c>
+      <c r="K23">
+        <v>0.2368421052631579</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>0.3829787234042553</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>164</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24">
+        <v>2.5</v>
+      </c>
+      <c r="E24">
+        <v>410</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>35</v>
+      </c>
+      <c r="J24">
+        <v>0.3</v>
+      </c>
+      <c r="K24">
+        <v>0.07894736842105263</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>0.1463414634146341</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>164</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>492</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>12</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>35</v>
+      </c>
+      <c r="J25">
+        <v>0.3</v>
+      </c>
+      <c r="K25">
+        <v>0.07894736842105263</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>0.1463414634146341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <v>164</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26">
+        <v>3.5</v>
+      </c>
+      <c r="E26">
+        <v>574</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>12</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>38</v>
+      </c>
+      <c r="J26">
+        <v>0.24</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>164</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>656</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>12</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>38</v>
+      </c>
+      <c r="J27">
+        <v>0.24</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>164</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28">
+        <v>4.5</v>
+      </c>
+      <c r="E28">
+        <v>738</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>12</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>38</v>
+      </c>
+      <c r="J28">
+        <v>0.24</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>164</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>820</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>38</v>
+      </c>
+      <c r="J29">
+        <v>0.24</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>164</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30">
+        <v>5.5</v>
+      </c>
+      <c r="E30">
         <v>902</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>12</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
         <v>38</v>
       </c>
-      <c r="J4">
+      <c r="J30">
         <v>0.24</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>0.9528508771929824</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31">
         <v>164</v>
       </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5">
-        <v>0.1</v>
-      </c>
-      <c r="E5">
-        <v>16.4</v>
-      </c>
-      <c r="F5">
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>984</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>12</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <v>38</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
+      <c r="J31">
+        <v>0.24</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>164</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32">
+        <v>6.5</v>
+      </c>
+      <c r="E32">
+        <v>1066</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
         <v>12</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0.76</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0.76</v>
-      </c>
-      <c r="N5">
-        <v>0.8636363636363636</v>
-      </c>
-      <c r="O5">
-        <v>0.9528508771929824</v>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>38</v>
+      </c>
+      <c r="J32">
+        <v>0.24</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>164</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>1148</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>12</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>38</v>
+      </c>
+      <c r="J33">
+        <v>0.24</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5778,18 +6956,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:AA48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5799,302 +6977,498 @@
       <c r="C2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>0.052632</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>85</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>0.184211</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>136</v>
+      </c>
+      <c r="D5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="B6">
-        <v>0.289474</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="C6">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>170</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7">
-        <v>0.368421</v>
+        <v>0.2894736842105263</v>
       </c>
       <c r="C7">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>255</v>
+      </c>
+      <c r="D7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8">
+        <v>0.2894736842105263</v>
+      </c>
+      <c r="C8">
+        <v>340</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="C9">
+        <v>425</v>
+      </c>
+      <c r="D9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>510</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>595</v>
+      </c>
+      <c r="D11">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>680</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>765</v>
+      </c>
+      <c r="D13">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>850</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>935</v>
+      </c>
+      <c r="D15">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1020</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1105</v>
+      </c>
+      <c r="D17">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1190</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>16.4</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>82</v>
+      </c>
+      <c r="D24">
         <v>0.5</v>
       </c>
-      <c r="C8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0.684211</v>
-      </c>
-      <c r="C9">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0.947368</v>
-      </c>
-      <c r="C10">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>0.166667</v>
-      </c>
-      <c r="B11">
-        <v>0.947368</v>
-      </c>
-      <c r="C11">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>0.166667</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>0.078947</v>
-      </c>
-      <c r="C19">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0.236842</v>
-      </c>
-      <c r="C20">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>0.289474</v>
-      </c>
-      <c r="C21">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>0.421053</v>
-      </c>
-      <c r="C22">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>0.526316</v>
-      </c>
-      <c r="C23">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>0.657895</v>
-      </c>
-      <c r="C24">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25">
-        <v>0.710526</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>131.2</v>
+      </c>
+      <c r="D25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="B26">
-        <v>0.868421</v>
+        <v>0.868421052631579</v>
       </c>
       <c r="C26">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>164</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
-        <v>0.166667</v>
+        <v>0</v>
       </c>
       <c r="B27">
-        <v>0.868421</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="C27">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>246</v>
+      </c>
+      <c r="D27">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
-        <v>0.333333</v>
+        <v>0</v>
       </c>
       <c r="B28">
-        <v>0.973684</v>
+        <v>0.2368421052631579</v>
       </c>
       <c r="C28">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>328</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
-        <v>0.583333</v>
+        <v>0</v>
       </c>
       <c r="B29">
-        <v>0.973684</v>
+        <v>0.07894736842105263</v>
       </c>
       <c r="C29">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>410</v>
+      </c>
+      <c r="D29">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0.07894736842105263</v>
       </c>
       <c r="C30">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="11:12">
-      <c r="K38" t="s">
-        <v>89</v>
-      </c>
-      <c r="L38" t="s">
+        <v>492</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>574</v>
+      </c>
+      <c r="D31">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>656</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>738</v>
+      </c>
+      <c r="D33">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>820</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>902</v>
+      </c>
+      <c r="D35">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>984</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>1066</v>
+      </c>
+      <c r="D37">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>1148</v>
+      </c>
+      <c r="D38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27">
+      <c r="Z46" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="39" spans="11:12">
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="11:12">
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40">
+      <c r="AA46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27">
+      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27">
+      <c r="Z48">
+        <v>1</v>
+      </c>
+      <c r="AA48">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved optimal z logic
</commit_message>
<xml_diff>
--- a/output/ROC Curve 2 Compounds_processed_analysis.xlsx
+++ b/output/ROC Curve 2 Compounds_processed_analysis.xlsx
@@ -5739,7 +5739,7 @@
         <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4">
         <v>0.8</v>
@@ -5783,7 +5783,7 @@
         <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D5">
         <v>1</v>

</xml_diff>